<commit_message>
Adding more performance numbers.
</commit_message>
<xml_diff>
--- a/test/PerformanceNumbers.xlsx
+++ b/test/PerformanceNumbers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="1480" windowWidth="30840" windowHeight="17740" tabRatio="500"/>
+    <workbookView xWindow="1400" yWindow="1580" windowWidth="30840" windowHeight="17740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Small Data Set" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Scenario</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -82,14 +82,6 @@
   </si>
   <si>
     <t>Average run time (10 Users) - Inside NCI Network</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cannot be run</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cannot be run</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -486,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -524,14 +516,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="F2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>1</v>
@@ -545,6 +529,9 @@
       <c r="E3" s="2">
         <v>5161</v>
       </c>
+      <c r="F3" s="2">
+        <v>17107</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
@@ -559,6 +546,9 @@
       <c r="E4" s="2">
         <v>3624</v>
       </c>
+      <c r="F4" s="2">
+        <v>7385</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
@@ -573,6 +563,9 @@
       <c r="E5" s="2">
         <v>4899</v>
       </c>
+      <c r="F5" s="2">
+        <v>8422</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
@@ -595,6 +588,9 @@
       <c r="E7" s="2">
         <v>6508</v>
       </c>
+      <c r="F7" s="2">
+        <v>24064</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
@@ -608,6 +604,9 @@
       </c>
       <c r="E8" s="2">
         <v>9173</v>
+      </c>
+      <c r="F8" s="2">
+        <v>36568</v>
       </c>
     </row>
     <row r="9" spans="1:7">

</xml_diff>